<commit_message>
translate Japanese to English.
</commit_message>
<xml_diff>
--- a/src/test/resources/example/DatastoreInfo.xlsx
+++ b/src/test/resources/example/DatastoreInfo.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>UTF-8</t>
     <phoneticPr fontId="1"/>
@@ -46,48 +46,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ファイル文字コード</t>
-    <rPh sb="4" eb="6">
-      <t>モジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>データストア名</t>
-    <rPh sb="6" eb="7">
-      <t>メイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タイプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>区切り文字</t>
-    <rPh sb="0" eb="2">
-      <t>クギ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>モジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>引用符</t>
-    <rPh sb="0" eb="3">
-      <t>インヨウフ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>改行コード</t>
-    <rPh sb="0" eb="2">
-      <t>カイギョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>\r\n</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -96,10 +54,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ディレクトリパス</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>TargetFiles</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -112,107 +66,122 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>\t</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>\"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>\'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>\r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>\n</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C:\tmp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Database</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>org.h2.Driver</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sa</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>jdbc:h2:mem:db_h2_002;DB_CLOSE_DELAY=-1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>jdbc:h2:mem:db_h2_001;DB_CLOSE_DELAY=-1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DB_H2_001</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DB_H2_002</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Datastore Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Datastore Type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DB User</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>JDBC Connection URL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>JDBC Driver Class</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DB Password</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DB Schema</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>File Directory Path</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>File Header</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Column Delimiter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Column Quate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>\r\n</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>,</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>文字コード</t>
-    <rPh sb="0" eb="2">
-      <t>モジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>\t</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>\"</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>\'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>\r</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>\n</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ヘッダ行</t>
-    <rPh sb="3" eb="4">
-      <t>ギョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>boolean</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DBユーザ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>JDBC接続URL</t>
-    <rPh sb="4" eb="6">
-      <t>セツゾク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DBパスワード</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DBスキーマ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>JDBCドライバクラス</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>C:\tmp</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Database</t>
-  </si>
-  <si>
-    <t>Database</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>org.h2.Driver</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>sa</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>jdbc:h2:mem:db_h2_002;DB_CLOSE_DELAY=-1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>jdbc:h2:mem:db_h2_001;DB_CLOSE_DELAY=-1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DB_H2_001</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DB_H2_002</t>
+    <t>Line Separator</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Codepage</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Boolean</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -322,7 +291,22 @@
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -624,34 +608,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.625" customWidth="1"/>
     <col min="3" max="3" width="18.875" customWidth="1"/>
-    <col min="4" max="4" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.625" customWidth="1"/>
-    <col min="8" max="8" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.125" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>27</v>
@@ -660,28 +644,28 @@
         <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
@@ -697,17 +681,17 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="M2" s="1" t="b">
         <v>1</v>
@@ -715,10 +699,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -726,17 +710,17 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="M3" s="1" t="b">
         <v>1</v>
@@ -744,19 +728,19 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -769,19 +753,19 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1259,6 +1243,16 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
+  <conditionalFormatting sqref="C2:G36">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$B2="LocalFile"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:M36">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$B2="Database"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B36">
       <formula1>タイプ</formula1>
@@ -1289,35 +1283,36 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
@@ -1328,11 +1323,11 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F2" s="3" t="b">
         <v>1</v>
@@ -1340,16 +1335,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>0</v>
@@ -1357,10 +1352,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support data sort before assertion.
</commit_message>
<xml_diff>
--- a/src/test/resources/example/DatastoreInfo.xlsx
+++ b/src/test/resources/example/DatastoreInfo.xlsx
@@ -17,171 +17,200 @@
   </sheets>
   <definedNames>
     <definedName name="boolean">Names!$F$2:$F$3</definedName>
-    <definedName name="タイプ">Names!$A$2:$A$3</definedName>
+    <definedName name="タイプ">Names!$A$2:$A$4</definedName>
     <definedName name="引用符">Names!$D$2:$D$4</definedName>
     <definedName name="改行コード">Names!$E$2:$E$4</definedName>
     <definedName name="区切り文字">Names!$C$2:$C$3</definedName>
-    <definedName name="文字コード">Names!$B$2</definedName>
+    <definedName name="文字コード">Names!$B$2:$B$3</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>UTF-8</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>UTF-8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>\r\n</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>UTF-8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>\t</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>\"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>\'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>\r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>\n</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C:\tmp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Database</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>org.h2.Driver</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sa</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>jdbc:h2:mem:db_h2_002;DB_CLOSE_DELAY=-1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>jdbc:h2:mem:db_h2_001;DB_CLOSE_DELAY=-1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DB_H2_001</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DB_H2_002</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Datastore Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Datastore Type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DB User</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>JDBC Connection URL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>JDBC Driver Class</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DB Password</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DB Schema</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>File Directory Path</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>File Header</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Column Delimiter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Column Quate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>\r\n</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Line Separator</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Codepage</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Boolean</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LocalFileFromExcel</t>
+  </si>
+  <si>
+    <t>LocalFileFromExcel</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MS932</t>
+  </si>
+  <si>
+    <t>MS932</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>LocalFile</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>SourceFiles</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>UTF-8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>\r\n</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>,</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>TargetFiles</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>LocalFile</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>UTF-8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>,</t>
+    <t>SourceFiles_CSV_UTF-8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TargetFiles_CSV_UTF-8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SourceFiles_TSV_MS932</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TargetFiles_TSV_MS932</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>\t</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>\"</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>\'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>\r</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>\n</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>C:\tmp</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Database</t>
-  </si>
-  <si>
-    <t>Database</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>org.h2.Driver</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>sa</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>jdbc:h2:mem:db_h2_002;DB_CLOSE_DELAY=-1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>jdbc:h2:mem:db_h2_001;DB_CLOSE_DELAY=-1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DB_H2_001</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DB_H2_002</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Datastore Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Datastore Type</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DB User</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>JDBC Connection URL</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>JDBC Driver Class</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DB Password</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DB Schema</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>File Directory Path</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>File Header</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Column Delimiter</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Column Quate</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>\r\n</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Line Separator</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Codepage</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Boolean</t>
+  </si>
+  <si>
+    <t>"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -291,7 +320,21 @@
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -606,13 +649,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.625" customWidth="1"/>
     <col min="3" max="3" width="18.875" customWidth="1"/>
     <col min="4" max="4" width="40.875" bestFit="1" customWidth="1"/>
@@ -629,51 +674,51 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -681,17 +726,19 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="L2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M2" s="1" t="b">
         <v>1</v>
@@ -699,10 +746,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -710,17 +757,19 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="L3" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="M3" s="1" t="b">
         <v>1</v>
@@ -728,60 +777,78 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
+      <c r="L5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -792,11 +859,21 @@
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1241,35 +1318,75 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="C2:G36">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$B2="LocalFile"</formula>
+  <conditionalFormatting sqref="C2:G38">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>$B2="LocalFileFromExcel"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:M36">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="H2:M38">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$B2="Database"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C4:G5">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$B4="LocalFile"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:M5">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$B4="Database"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B38">
       <formula1>タイプ</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I38">
       <formula1>文字コード</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J38">
       <formula1>区切り文字</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K38">
       <formula1>引用符</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L38">
       <formula1>改行コード</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M38">
       <formula1>boolean</formula1>
     </dataValidation>
   </dataValidations>
@@ -1283,7 +1400,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1297,37 +1414,37 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2" s="3" t="b">
         <v>1</v>
@@ -1335,27 +1452,33 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add flat file support
</commit_message>
<xml_diff>
--- a/src/test/resources/example/DatastoreInfo.xlsx
+++ b/src/test/resources/example/DatastoreInfo.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
   <si>
     <t>UTF-8</t>
     <phoneticPr fontId="1"/>
@@ -74,10 +74,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>C:\tmp</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Database</t>
   </si>
   <si>
@@ -211,6 +207,35 @@
   </si>
   <si>
     <t>"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LocalFile</t>
+  </si>
+  <si>
+    <t>UTF-8</t>
+  </si>
+  <si>
+    <t>SourceFiles_MS932</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TargetFiles_MS932</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SourceFiles_UTF-8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TargetFiles_UTF-8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C:/tmp</t>
+  </si>
+  <si>
+    <t>C:/tmp</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -320,7 +345,35 @@
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -649,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -674,51 +727,51 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -726,7 +779,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>1</v>
@@ -735,7 +788,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>2</v>
@@ -746,10 +799,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -757,7 +810,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>4</v>
@@ -766,10 +819,10 @@
         <v>5</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M3" s="1" t="b">
         <v>1</v>
@@ -777,10 +830,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -788,13 +841,13 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
@@ -806,10 +859,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -817,17 +870,17 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M5" s="1" t="b">
         <v>1</v>
@@ -835,19 +888,19 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -860,19 +913,19 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -884,60 +937,92 @@
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1348,45 +1433,85 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
     </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="C2:G38">
-    <cfRule type="expression" dxfId="3" priority="4">
+  <conditionalFormatting sqref="C2:G7 C10:G40">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>$B2="LocalFileFromExcel"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:M38">
-    <cfRule type="expression" dxfId="2" priority="3">
+  <conditionalFormatting sqref="H2:M7 H10:M40">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>$B2="Database"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:G5">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>$B4="LocalFile"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:M5">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$B4="Database"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C8:G9">
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>$B8="LocalFileFromExcel"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8:M9">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>$B8="Database"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B38">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B40">
       <formula1>タイプ</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I38">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I40">
       <formula1>文字コード</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J38">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J40">
       <formula1>区切り文字</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K38">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K40">
       <formula1>引用符</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L38">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L40">
       <formula1>改行コード</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M38">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M40">
       <formula1>boolean</formula1>
     </dataValidation>
   </dataValidations>
@@ -1414,27 +1539,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -1452,10 +1577,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -1472,7 +1597,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>

</xml_diff>